<commit_message>
Changes made based on new data
</commit_message>
<xml_diff>
--- a/src/test/resources/documents/Data.xlsx
+++ b/src/test/resources/documents/Data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
@@ -467,7 +467,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E69CF920-E52B-4762-BB13-A8AFC7F07B32}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
@@ -528,6 +528,28 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>300.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>